<commit_message>
changes to preface, outline and last changes training, ready for first review
</commit_message>
<xml_diff>
--- a/docs/resources/skill-matrix.xlsx
+++ b/docs/resources/skill-matrix.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Dropbox\g2sq\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/projects/g2sq/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42B8E65-2B03-4875-A0CF-730D95935CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BBCE73-8860-CB48-8900-4B75D4799D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B16051D-53AA-414D-BBBB-4D5CDC4D4C8F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="26000" windowHeight="12880" xr2:uid="{8B16051D-53AA-414D-BBBB-4D5CDC4D4C8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Sunday</t>
   </si>
@@ -130,6 +133,11 @@
   </si>
   <si>
     <t>needs help with CAPI, OK in interviewing</t>
+  </si>
+  <si>
+    <t>- navigation
+- completion checks
+- assignments &amp; sync</t>
   </si>
 </sst>
 </file>
@@ -210,12 +218,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -232,10 +234,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -550,102 +558,103 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="5.88671875" customWidth="1"/>
-    <col min="8" max="14" width="5.77734375" customWidth="1"/>
+    <col min="6" max="14" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:14" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="10">
+      <c r="E3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="8">
         <v>9</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>8</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -673,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -701,7 +710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -726,7 +735,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -754,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -776,7 +785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -804,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -832,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -863,7 +872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -894,7 +903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -922,7 +931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>

</xml_diff>